<commit_message>
Gravação Aula 5 6
</commit_message>
<xml_diff>
--- a/dadosDaTabela.xlsx
+++ b/dadosDaTabela.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/500ae9e30167d4d4/Documentos/UiPath/FormatadorDePlanilha/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{8A61B5D6-2491-4ABD-9CF0-CD7AFC0DEB99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0D61E3E6-D354-4DB8-AF4F-A48EC24FCAEC}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{8A61B5D6-2491-4ABD-9CF0-CD7AFC0DEB99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EC5EFD50-6157-402C-966F-B9243A57C799}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="2025" windowWidth="18000" windowHeight="9360" xr2:uid="{D2E589DF-E358-46D7-9327-AD7460D5E8B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{D2E589DF-E358-46D7-9327-AD7460D5E8B4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dados Filtrados" sheetId="3" r:id="rId1"/>
-    <sheet name="Dados Extraidos" sheetId="2" r:id="rId2"/>
+    <sheet name="Dados Extraidos" sheetId="2" r:id="rId1"/>
+    <sheet name="Dados Filtrados" sheetId="5" r:id="rId2"/>
+    <sheet name="Dados Filtrados 2" sheetId="6" r:id="rId3"/>
+    <sheet name="Dados Filtrados 3" sheetId="7" r:id="rId4"/>
+    <sheet name="Dados Filtrados 4" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="16">
   <si>
     <t>Research Client Check Copy</t>
   </si>
@@ -104,12 +107,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -133,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -145,6 +154,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,704 +468,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C317DD34-9396-4874-A290-133BE44038E9}">
-  <dimension ref="A1:E40"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>59081375</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4">
-        <v>43834</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>59081400</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4">
-        <v>42974</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>59081390</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4">
-        <v>42831</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>59081392</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4">
-        <v>42837</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>59081379</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4">
-        <v>43072</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>59081412</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4">
-        <v>43978</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>59081406</v>
-      </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4">
-        <v>42790</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>59081408</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="4">
-        <v>43903</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>59081391</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4">
-        <v>43422</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>59081411</v>
-      </c>
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="4">
-        <v>43292</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>59081410</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4">
-        <v>42999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>59081407</v>
-      </c>
-      <c r="B12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4">
-        <v>43953</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>59081393</v>
-      </c>
-      <c r="B13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4">
-        <v>43072</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>59081378</v>
-      </c>
-      <c r="B14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="4">
-        <v>43670</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>59081404</v>
-      </c>
-      <c r="B15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="4">
-        <v>43042</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>59081377</v>
-      </c>
-      <c r="B16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="4">
-        <v>43453</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>59081401</v>
-      </c>
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="4">
-        <v>43096</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>59081381</v>
-      </c>
-      <c r="B18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="4">
-        <v>42905</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>59081394</v>
-      </c>
-      <c r="B19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="4">
-        <v>43448</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>59081380</v>
-      </c>
-      <c r="B20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="4">
-        <v>42784</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>59081382</v>
-      </c>
-      <c r="B21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="4">
-        <v>44019</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>59081397</v>
-      </c>
-      <c r="B22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="4">
-        <v>43912</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>59081389</v>
-      </c>
-      <c r="B23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="4">
-        <v>43594</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>59081383</v>
-      </c>
-      <c r="B24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>2</v>
-      </c>
-      <c r="E24" s="4">
-        <v>42795</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>59081384</v>
-      </c>
-      <c r="B25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" s="4">
-        <v>43583</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>59081376</v>
-      </c>
-      <c r="B26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" s="4">
-        <v>43634</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>59081409</v>
-      </c>
-      <c r="B27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>2</v>
-      </c>
-      <c r="E27" s="4">
-        <v>43904</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>59081398</v>
-      </c>
-      <c r="B28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="4">
-        <v>43268</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>59081387</v>
-      </c>
-      <c r="B29" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" s="4">
-        <v>43601</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>59081403</v>
-      </c>
-      <c r="B30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="4">
-        <v>43868</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>59081396</v>
-      </c>
-      <c r="B31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" s="4">
-        <v>42786</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>59081399</v>
-      </c>
-      <c r="B32" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" s="4">
-        <v>42824</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>59081385</v>
-      </c>
-      <c r="B33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>2</v>
-      </c>
-      <c r="E33" s="4">
-        <v>43508</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>59081414</v>
-      </c>
-      <c r="B34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>2</v>
-      </c>
-      <c r="E34" s="4">
-        <v>43794</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>59081413</v>
-      </c>
-      <c r="B35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" t="s">
-        <v>2</v>
-      </c>
-      <c r="E35" s="4">
-        <v>43703</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>59081405</v>
-      </c>
-      <c r="B36" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>2</v>
-      </c>
-      <c r="E36" s="4">
-        <v>43447</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>59081388</v>
-      </c>
-      <c r="B37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>2</v>
-      </c>
-      <c r="E37" s="4">
-        <v>43727</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>59081402</v>
-      </c>
-      <c r="B38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
-        <v>2</v>
-      </c>
-      <c r="E38" s="4">
-        <v>42746</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>59081395</v>
-      </c>
-      <c r="B39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>2</v>
-      </c>
-      <c r="E39" s="4">
-        <v>43964</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>59081386</v>
-      </c>
-      <c r="B40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" t="s">
-        <v>2</v>
-      </c>
-      <c r="E40" s="4">
-        <v>42773</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D3FEB9-6AD6-49B8-9E41-C975C6BBFEC9}">
   <dimension ref="A1:E126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3314,4 +2631,2084 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D411BA-E928-4DB5-95A6-9C9E757B6F72}">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>59081375</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4">
+        <v>43834</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>59081400</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>42974</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>59081390</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>42831</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>59081392</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>42837</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>59081379</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>43072</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>59081412</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>43978</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>59081406</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>42790</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>59081408</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4">
+        <v>43903</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>59081391</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4">
+        <v>43422</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>59081411</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="4">
+        <v>43292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>59081410</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>42999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>59081407</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4">
+        <v>43953</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>59081393</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="4">
+        <v>43072</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>59081378</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4">
+        <v>43670</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>59081404</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4">
+        <v>43042</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>59081377</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="4">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>59081401</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="4">
+        <v>43096</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>59081381</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="4">
+        <v>42905</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>59081394</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4">
+        <v>43448</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>59081380</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="4">
+        <v>42784</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>59081382</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4">
+        <v>44019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>59081397</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="4">
+        <v>43912</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>59081389</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4">
+        <v>43594</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>59081383</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="4">
+        <v>42795</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>59081384</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4">
+        <v>43583</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>59081376</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="4">
+        <v>43634</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>59081409</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="4">
+        <v>43904</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>59081398</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="4">
+        <v>43268</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>59081387</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="4">
+        <v>43601</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>59081403</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="4">
+        <v>43868</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>59081396</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="4">
+        <v>42786</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>59081399</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="4">
+        <v>42824</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>59081385</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="4">
+        <v>43508</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>59081414</v>
+      </c>
+      <c r="B34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="4">
+        <v>43794</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>59081413</v>
+      </c>
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="4">
+        <v>43703</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>59081405</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="4">
+        <v>43447</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>59081388</v>
+      </c>
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="4">
+        <v>43727</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>59081402</v>
+      </c>
+      <c r="B38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="4">
+        <v>42746</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>59081395</v>
+      </c>
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" s="4">
+        <v>43964</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>59081386</v>
+      </c>
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" s="4">
+        <v>42773</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0944B08-C824-40FA-B373-F99B215512C5}">
+  <dimension ref="A1:A40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4">
+        <v>43834</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>42974</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>42831</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>42837</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>43072</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>43978</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>42790</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>43903</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>43422</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>43292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>42999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>43953</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>43072</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>43670</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>43042</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>43453</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>43096</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>42905</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>43448</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>42784</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>44019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>43912</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>43594</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>42795</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>43583</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>43634</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>43904</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>43268</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>43601</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>43868</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>42786</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>42824</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>43508</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>43794</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>43703</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>43447</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>43727</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>42746</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>43964</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>42773</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850415A2-FA30-49B0-93AF-6A05413DF160}">
+  <dimension ref="A1:D40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>59081375</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>59081400</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>59081390</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>59081392</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>59081379</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>59081412</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>59081406</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>59081408</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>59081391</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>59081411</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>59081410</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>59081407</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>59081393</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>59081378</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>59081404</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>59081377</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>59081401</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>59081381</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>59081394</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>59081380</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>59081382</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>59081397</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>59081389</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>59081383</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>59081384</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>59081376</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>59081409</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>59081398</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>59081387</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>59081403</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>59081396</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>59081399</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>59081385</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>59081414</v>
+      </c>
+      <c r="B34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>59081413</v>
+      </c>
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>59081405</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>59081388</v>
+      </c>
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>59081402</v>
+      </c>
+      <c r="B38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>59081395</v>
+      </c>
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>59081386</v>
+      </c>
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35CC1448-8F75-4BB3-8971-81CE2A7581D1}">
+  <dimension ref="A1:D40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5">
+        <v>59081375</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>59081400</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>59081390</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>59081392</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>59081379</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>59081412</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>59081406</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>59081408</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>59081391</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>59081411</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>59081410</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>59081407</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>59081393</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>59081378</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>59081404</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>59081377</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>59081401</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>59081381</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>59081394</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>59081380</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>59081382</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>59081397</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>59081389</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>59081383</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>59081384</v>
+      </c>
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>59081376</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>59081409</v>
+      </c>
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>59081398</v>
+      </c>
+      <c r="B28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>59081387</v>
+      </c>
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>59081403</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>59081396</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>59081399</v>
+      </c>
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>59081385</v>
+      </c>
+      <c r="B33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>59081414</v>
+      </c>
+      <c r="B34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>59081413</v>
+      </c>
+      <c r="B35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>59081405</v>
+      </c>
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>59081388</v>
+      </c>
+      <c r="B37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>59081402</v>
+      </c>
+      <c r="B38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>59081395</v>
+      </c>
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>59081386</v>
+      </c>
+      <c r="B40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>